<commit_message>
changed bom, one wrong part, some out of stock at time of order
</commit_message>
<xml_diff>
--- a/phasefreq-bom.xlsx
+++ b/phasefreq-bom.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bob Peterson\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bob Peterson\ucloud\Shared\Quantum Photonics Group\3D Design\Gravity\phasefreq\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -375,9 +375,6 @@
     <t>https://www.digikey.at/product-detail/en/avx-corporation/F931A476KAA/478-8223-1-ND/4005652</t>
   </si>
   <si>
-    <t>https://www.digikey.at/product-detail/en/avx-corporation/TACL475K010RTA/478-7523-1-ND/3660395</t>
-  </si>
-  <si>
     <t>https://www.digikey.at/product-detail/en/avx-corporation/TACL105K010RTA/478-7521-1-ND/3660394</t>
   </si>
   <si>
@@ -405,9 +402,6 @@
     <t>https://www.digikey.at/product-detail/en/analog-devices-inc/AD9901KPZ/AD9901KPZ-ND/820034</t>
   </si>
   <si>
-    <t>https://www.digikey.at/product-detail/en/texas-instruments/REF1925AIDDCT/296-38442-1-ND/5015866</t>
-  </si>
-  <si>
     <t>https://www.digikey.at/product-detail/en/analog-devices-inc/AD8676ARZ-REEL7/AD8676ARZ-REEL7CT-ND/3828889</t>
   </si>
   <si>
@@ -469,6 +463,12 @@
   </si>
   <si>
     <t>https://www.digikey.at/product-detail/en/vishay-beyschlag/MCT06030Z0000ZP500/MCT0603-0.0-ZZCT-ND/2607921</t>
+  </si>
+  <si>
+    <t>https://www.digikey.at/product-detail/en/diodes-incorporated/LM4040C25FTA/LM4040C25FCT-ND/1557754</t>
+  </si>
+  <si>
+    <t>https://www.digikey.at/product-detail/en/avx-corporation/TPCL475K010R5000/478-4961-1-ND/1879558</t>
   </si>
 </sst>
 </file>
@@ -1323,7 +1323,7 @@
   <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1452,7 +1452,7 @@
         <v/>
       </c>
       <c r="H8" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -1506,7 +1506,7 @@
         <v/>
       </c>
       <c r="H10" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -1533,7 +1533,7 @@
         <v/>
       </c>
       <c r="H11" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -1560,7 +1560,7 @@
         <v/>
       </c>
       <c r="H12" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -1587,7 +1587,7 @@
         <v/>
       </c>
       <c r="H13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -1614,7 +1614,7 @@
         <v/>
       </c>
       <c r="H14" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -1636,12 +1636,8 @@
       <c r="F15" t="s">
         <v>19</v>
       </c>
-      <c r="G15" t="str">
-        <f>""</f>
-        <v/>
-      </c>
       <c r="H15" s="4" t="s">
-        <v>118</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -1668,7 +1664,7 @@
         <v/>
       </c>
       <c r="H16" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -1695,7 +1691,7 @@
         <v/>
       </c>
       <c r="H17" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -1722,7 +1718,7 @@
         <v/>
       </c>
       <c r="H18" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -1749,7 +1745,7 @@
         <v/>
       </c>
       <c r="H19" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
@@ -1776,7 +1772,7 @@
         <v/>
       </c>
       <c r="H20" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -1803,7 +1799,7 @@
         <v/>
       </c>
       <c r="H21" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
@@ -1830,7 +1826,7 @@
         <v/>
       </c>
       <c r="H22" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
@@ -1857,7 +1853,7 @@
         <v/>
       </c>
       <c r="H23" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
@@ -1884,7 +1880,7 @@
         <v/>
       </c>
       <c r="H24" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
@@ -1911,7 +1907,7 @@
         <v/>
       </c>
       <c r="H25" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -1938,7 +1934,7 @@
         <v/>
       </c>
       <c r="H26" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
@@ -1965,7 +1961,7 @@
         <v/>
       </c>
       <c r="H27" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
@@ -1992,7 +1988,7 @@
         <v/>
       </c>
       <c r="H28" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
@@ -2019,7 +2015,7 @@
         <v/>
       </c>
       <c r="H29" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
@@ -2046,7 +2042,7 @@
         <v/>
       </c>
       <c r="H30" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
@@ -2073,7 +2069,7 @@
         <v/>
       </c>
       <c r="H31" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
@@ -2100,7 +2096,7 @@
         <v/>
       </c>
       <c r="H32" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
@@ -2127,7 +2123,7 @@
         <v/>
       </c>
       <c r="H33" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
@@ -2149,12 +2145,8 @@
       <c r="F34" t="s">
         <v>66</v>
       </c>
-      <c r="G34" t="str">
-        <f>""</f>
-        <v/>
-      </c>
       <c r="H34" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2181,7 +2173,7 @@
         <v/>
       </c>
       <c r="H35" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
@@ -2208,7 +2200,7 @@
         <v/>
       </c>
       <c r="H36" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
@@ -2235,7 +2227,7 @@
         <v/>
       </c>
       <c r="H37" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
@@ -2262,7 +2254,7 @@
         <v/>
       </c>
       <c r="H38" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
@@ -2289,7 +2281,7 @@
         <v/>
       </c>
       <c r="H39" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
@@ -2313,7 +2305,7 @@
         <v/>
       </c>
       <c r="H40" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
@@ -2332,12 +2324,8 @@
       <c r="E41" t="s">
         <v>107</v>
       </c>
-      <c r="G41" t="str">
-        <f>""</f>
-        <v/>
-      </c>
       <c r="H41" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
@@ -2359,12 +2347,8 @@
       <c r="F42" t="s">
         <v>112</v>
       </c>
-      <c r="G42" t="str">
-        <f>""</f>
-        <v/>
-      </c>
       <c r="H42" s="4" t="s">
-        <v>128</v>
+        <v>148</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
@@ -2384,7 +2368,7 @@
         <v>41</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -2396,38 +2380,36 @@
   <hyperlinks>
     <hyperlink ref="H7" r:id="rId1"/>
     <hyperlink ref="H9" r:id="rId2"/>
-    <hyperlink ref="H15" r:id="rId3"/>
-    <hyperlink ref="H11" r:id="rId4"/>
-    <hyperlink ref="H16" r:id="rId5"/>
-    <hyperlink ref="H17" r:id="rId6"/>
-    <hyperlink ref="H19" r:id="rId7"/>
-    <hyperlink ref="H37" r:id="rId8"/>
-    <hyperlink ref="H38" r:id="rId9"/>
-    <hyperlink ref="H39" r:id="rId10"/>
-    <hyperlink ref="H40" r:id="rId11"/>
-    <hyperlink ref="H41" r:id="rId12"/>
-    <hyperlink ref="H42" r:id="rId13"/>
-    <hyperlink ref="H43" r:id="rId14"/>
-    <hyperlink ref="H14" r:id="rId15"/>
-    <hyperlink ref="H10" r:id="rId16"/>
-    <hyperlink ref="H8" r:id="rId17"/>
-    <hyperlink ref="H12" r:id="rId18"/>
-    <hyperlink ref="H24" r:id="rId19"/>
-    <hyperlink ref="H28" r:id="rId20"/>
-    <hyperlink ref="H22" r:id="rId21"/>
-    <hyperlink ref="H30" r:id="rId22"/>
-    <hyperlink ref="H23" r:id="rId23"/>
-    <hyperlink ref="H31" r:id="rId24"/>
-    <hyperlink ref="H35" r:id="rId25"/>
-    <hyperlink ref="H36" r:id="rId26"/>
-    <hyperlink ref="H34" r:id="rId27"/>
-    <hyperlink ref="H29" r:id="rId28"/>
-    <hyperlink ref="H25" r:id="rId29"/>
-    <hyperlink ref="H26" r:id="rId30"/>
-    <hyperlink ref="H27" r:id="rId31"/>
-    <hyperlink ref="H32" r:id="rId32"/>
+    <hyperlink ref="H11" r:id="rId3"/>
+    <hyperlink ref="H16" r:id="rId4"/>
+    <hyperlink ref="H17" r:id="rId5"/>
+    <hyperlink ref="H19" r:id="rId6"/>
+    <hyperlink ref="H37" r:id="rId7"/>
+    <hyperlink ref="H38" r:id="rId8"/>
+    <hyperlink ref="H39" r:id="rId9"/>
+    <hyperlink ref="H40" r:id="rId10"/>
+    <hyperlink ref="H41" r:id="rId11"/>
+    <hyperlink ref="H43" r:id="rId12"/>
+    <hyperlink ref="H14" r:id="rId13"/>
+    <hyperlink ref="H10" r:id="rId14"/>
+    <hyperlink ref="H8" r:id="rId15"/>
+    <hyperlink ref="H12" r:id="rId16"/>
+    <hyperlink ref="H24" r:id="rId17"/>
+    <hyperlink ref="H28" r:id="rId18"/>
+    <hyperlink ref="H22" r:id="rId19"/>
+    <hyperlink ref="H30" r:id="rId20"/>
+    <hyperlink ref="H23" r:id="rId21"/>
+    <hyperlink ref="H31" r:id="rId22"/>
+    <hyperlink ref="H35" r:id="rId23"/>
+    <hyperlink ref="H36" r:id="rId24"/>
+    <hyperlink ref="H34" r:id="rId25"/>
+    <hyperlink ref="H29" r:id="rId26"/>
+    <hyperlink ref="H25" r:id="rId27"/>
+    <hyperlink ref="H26" r:id="rId28"/>
+    <hyperlink ref="H27" r:id="rId29"/>
+    <hyperlink ref="H32" r:id="rId30"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId33"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId31"/>
 </worksheet>
 </file>
</xml_diff>